<commit_message>
BACKUP SAS BY PRINCE
</commit_message>
<xml_diff>
--- a/functions/templates/Upload New Employee.xlsx
+++ b/functions/templates/Upload New Employee.xlsx
@@ -768,7 +768,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G548"/>
+  <dimension ref="A1:G550"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -5835,6 +5835,24 @@
       <c r="E548"/>
       <c r="F548"/>
       <c r="G548"/>
+    </row>
+    <row r="549" spans="1:7">
+      <c r="A549"/>
+      <c r="B549" s="2"/>
+      <c r="C549"/>
+      <c r="D549" s="2"/>
+      <c r="E549"/>
+      <c r="F549"/>
+      <c r="G549"/>
+    </row>
+    <row r="550" spans="1:7">
+      <c r="A550"/>
+      <c r="B550" s="2"/>
+      <c r="C550"/>
+      <c r="D550" s="2"/>
+      <c r="E550"/>
+      <c r="F550"/>
+      <c r="G550"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>